<commit_message>
Modification GeolAssets and LG_GeolAssets
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V1_JM.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V1_JM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="884" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="884" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -2122,8 +2122,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5087857" y="855332"/>
-          <a:ext cx="13198561" cy="8532219"/>
+          <a:off x="5082085" y="855332"/>
+          <a:ext cx="13137946" cy="8529333"/>
           <a:chOff x="5327766" y="462648"/>
           <a:chExt cx="12988408" cy="8308516"/>
         </a:xfrm>
@@ -3659,8 +3659,8 @@
   </sheetPr>
   <dimension ref="A4:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="I9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+    <sheetView topLeftCell="H22" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5449,7 +5449,7 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -6532,7 +6532,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.90625" style="1"/>
+    <col min="1" max="4" width="10.90625" style="1"/>
+    <col min="5" max="5" width="52.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -7059,7 +7061,7 @@
   </sheetPr>
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adopte Catalogues -> Error for LG_GeolAssetsCatalogues
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V1_JM.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V1_JM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="884" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="884" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -2122,8 +2122,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5082085" y="855332"/>
-          <a:ext cx="13137946" cy="8529333"/>
+          <a:off x="5082662" y="853600"/>
+          <a:ext cx="13162192" cy="8505665"/>
           <a:chOff x="5327766" y="462648"/>
           <a:chExt cx="12988408" cy="8308516"/>
         </a:xfrm>
@@ -3659,7 +3659,7 @@
   </sheetPr>
   <dimension ref="A4:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="H22" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -5449,7 +5449,7 @@
   </sheetPr>
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -5630,7 +5630,7 @@
     <col min="1" max="1" width="10.90625" style="1"/>
     <col min="2" max="2" width="9.90625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.90625" style="1"/>
-    <col min="4" max="4" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
@@ -8613,7 +8613,7 @@
   </sheetPr>
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9115,7 +9115,7 @@
   </sheetPr>
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>

</xml_diff>